<commit_message>
Refactored project to prep for more organization when adding loading bar; fixed bug with max_col/max_row being wrong with new_wb
</commit_message>
<xml_diff>
--- a/samples/main.xlsx
+++ b/samples/main.xlsx
@@ -2253,10 +2253,10 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="D12" activeCellId="0" sqref="D12"/>
+      <selection pane="bottomLeft" activeCell="C13" activeCellId="0" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="13.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="1" width="12.14"/>

</xml_diff>

<commit_message>
Fixed issue where formatting would reset for newly added rows
</commit_message>
<xml_diff>
--- a/samples/main.xlsx
+++ b/samples/main.xlsx
@@ -2155,12 +2155,18 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFFF00"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -2197,7 +2203,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2208,6 +2214,22 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -2251,12 +2273,12 @@
   <dimension ref="A1:P1492"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A1478" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="P1492" activeCellId="0" sqref="P1492"/>
+      <selection pane="bottomLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="13.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="1" width="12.14"/>
@@ -2321,36 +2343,41 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+    <row r="2" customFormat="false" ht="60.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="E2" s="0"/>
-      <c r="F2" s="1" t="n">
+      <c r="E2" s="5"/>
+      <c r="F2" s="6" t="n">
         <v>653</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G2" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="H2" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="I2" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="O2" s="1" t="s">
+      <c r="J2" s="4"/>
+      <c r="K2" s="4"/>
+      <c r="L2" s="4"/>
+      <c r="M2" s="4"/>
+      <c r="N2" s="4"/>
+      <c r="O2" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="P2" s="1" t="s">
+      <c r="P2" s="4" t="s">
         <v>24</v>
       </c>
     </row>

</xml_diff>